<commit_message>
+ affichage des sous titres sur la vidéo !
</commit_message>
<xml_diff>
--- a/Bugs & Todo's.xlsx
+++ b/Bugs & Todo's.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmation\tauri\QuranCaption-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D50AD8-18FF-4922-9022-DC13C0FF0EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971B009C-C6D8-4FA9-9BEE-D55FEE71B7C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Id</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Faire en sorte de pouvoir sélectionner les mots du verset en maintenant le clique gauche enfoncé, comme si on sélectionné du texte. Demande d'utiliser mouseover (qui ne réagit pas comme click)</t>
+  </si>
+  <si>
+    <t>Pouvoir changer le sous-titre existant lorsqu'on sélectionne du texte dans une zone déjà sous-titré</t>
   </si>
 </sst>
 </file>
@@ -443,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,6 +512,72 @@
       </c>
       <c r="I2" s="6"/>
     </row>
+    <row r="3" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
bug fix (id: 2) => padding horizontal et hauteur du texte responsive à la taille de la vidéo !
</commit_message>
<xml_diff>
--- a/Bugs & Todo's.xlsx
+++ b/Bugs & Todo's.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmation\tauri\QuranCaption-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971B009C-C6D8-4FA9-9BEE-D55FEE71B7C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31189AFF-1E64-499B-A9D2-0433BEBA4B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Id</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>Pouvoir changer le sous-titre existant lorsqu'on sélectionne du texte dans une zone déjà sous-titré</t>
+  </si>
+  <si>
+    <t>Vertical Position &amp; Horizontal Padding ne s'adapte pas à la taille de la vidéo.</t>
+  </si>
+  <si>
+    <t>Corrigé le 16/06/2024</t>
   </si>
 </sst>
 </file>
@@ -448,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,6 +519,18 @@
       <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="F3" s="2">
         <v>2</v>
       </c>
@@ -525,42 +543,70 @@
       <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>

</xml_diff>

<commit_message>
+ page de translations / commencement de l'ajour des traductions
</commit_message>
<xml_diff>
--- a/Bugs & Todo's.xlsx
+++ b/Bugs & Todo's.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmation\tauri\QuranCaption-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31189AFF-1E64-499B-A9D2-0433BEBA4B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD59B03-5328-483E-99D9-D479A6A16697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>Id</t>
   </si>
@@ -64,6 +64,28 @@
   </si>
   <si>
     <t>Corrigé le 16/06/2024</t>
+  </si>
+  <si>
+    <t>GPT Prompt : Voici un verset en arabe et sa traduction :
+{
+verset: "وَٱتَّقُوا۟ يَوْمًۭا لَّا تَجْزِى نَفْسٌ عَن نَّفْسٍۢ شَيْـًۭٔا وَلَا يُقْبَلُ مِنْهَا عَدْلٌۭ وَلَا تَنفَعُهَا شَفَـٰعَةٌۭ وَلَا هُمْ يُنصَرُونَ",
+traduction: "Craignez le Jour où nul ne pourra rien pour son prochain, où nul ne pourra racheter son âme, nulle intercession ne sera acceptée sans l’autorisation d’Allah et nul ne pourra être sauvé s’il meurt dans l’impiété."
+}
+Maintenant je vais te donner le verset découpé en plusieurs morçeaux, et toi tu dois me donner la partie de la traduction correspondant à chaque morçeau. Par exemple, si je te donne :
+{
+versets: ["وَٱتَّقُوا۟ يَوْمًا لَّا تَجْزِى نَفْسٌ عَن نَّفْسٍ شَيْـًٔا","وَلَا يُقْبَلُ مِنْهَا عَدْلٌ وَلَا تَنفَعُهَا شَفَٰعَةٌ","وَلَا هُمْ يُنصَرُونَ"],
+traduction: "Craignez le Jour où nul ne pourra rien pour son prochain, où nul ne pourra racheter son âme, nulle intercession ne sera acceptée sans l’autorisation d’Allah et nul ne pourra être sauvé s’il meurt dans l’impiété."
+}
+tu dois me retourner, au format json :
+{
+traductions: ["Craignez le Jour où nul ne pourra rien pour son prochain, où nul ne pourra racheter son âme,","nulle intercession ne sera acceptée sans l’autorisation d’Allah","et nul ne pourra être sauvé s’il meurt dans l’impiété."]
+}
+Maintenant que je t'ai donné un exemple et expliqué ton travail, fait de meme avec cet input :
+{
+versets: ["قُلْ أَتُحَآجُّونَنَا فِى ٱللَّهِ", "وَهُوَ رَبُّنَا وَرَبُّكُمْ ", "وَلَنَآ أَعْمَٰلُنَا وَلَكُمْ أَعْمَٰلُكُمْ", "وَنَحْنُ لَهُۥ مُخْلِصُونَ"],
+traduction: "Dis: "Discutez-vous avec nous au sujet de Dieu, alors qu'Il est notre Seigneur et le vôtre? A nous nos actions et à vous les vôtres! C'est à Lui que nous sommes dévoués."
+}
+J'attends de toi 4 traductions car il y a 4 versets donnés.</t>
   </si>
 </sst>
 </file>
@@ -144,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -167,6 +189,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,6 +647,11 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
+ quelques modif de style
</commit_message>
<xml_diff>
--- a/Bugs & Todo's.xlsx
+++ b/Bugs & Todo's.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmation\tauri\QuranCaption-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD59B03-5328-483E-99D9-D479A6A16697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E30FE0C-CA65-4AEC-A629-C2B6A08E084C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Id</t>
   </si>
@@ -87,6 +87,12 @@
 }
 J'attends de toi 4 traductions car il y a 4 versets donnés.</t>
   </si>
+  <si>
+    <t>Fix l'UI !!! Dans la page translations et subtitles editors lorsqu'on sélectionne un très grand verset</t>
+  </si>
+  <si>
+    <t>À faire</t>
+  </si>
 </sst>
 </file>
 
@@ -101,7 +107,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,6 +141,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -189,7 +201,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,10 +579,16 @@
       </c>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+    <row r="4" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="D4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -648,7 +668,7 @@
       <c r="I12" s="2"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="A22" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>